<commit_message>
Prep for 0.2-6 release
Adding documentation, unit tests; adapting DESCRIPTION file
</commit_message>
<xml_diff>
--- a/inst/demoFiles/mtcars.xlsx
+++ b/inst/demoFiles/mtcars.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="750" yWindow="555" windowWidth="19815" windowHeight="7620"/>
+    <workbookView xWindow="750" yWindow="555" windowWidth="19815" windowHeight="7620" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="mtcars" sheetId="1" r:id="rId1"/>
     <sheet name="mtcars2" sheetId="2" r:id="rId2"/>
     <sheet name="mtcars3" sheetId="3" r:id="rId3"/>
+    <sheet name="mtcars_table" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="mtcars">mtcars!$A$1:$K$33</definedName>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="13">
   <si>
     <t>mpg</t>
   </si>
@@ -110,9 +111,87 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="13">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="MtcarsTable" displayName="MtcarsTable" ref="C5:M37" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+  <autoFilter ref="C5:M37"/>
+  <tableColumns count="11">
+    <tableColumn id="1" name="mpg" dataDxfId="12"/>
+    <tableColumn id="2" name="cyl" dataDxfId="11"/>
+    <tableColumn id="3" name="disp" dataDxfId="10"/>
+    <tableColumn id="4" name="hp" dataDxfId="9"/>
+    <tableColumn id="5" name="drat" dataDxfId="8"/>
+    <tableColumn id="6" name="wt" dataDxfId="7"/>
+    <tableColumn id="7" name="qsec" dataDxfId="6"/>
+    <tableColumn id="8" name="vs" dataDxfId="5"/>
+    <tableColumn id="9" name="am" dataDxfId="4"/>
+    <tableColumn id="10" name="gear" dataDxfId="3"/>
+    <tableColumn id="11" name="carb" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -402,8 +481,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection sqref="A1:K33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -3953,4 +4032,1178 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="C5:M37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="N15" sqref="N15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="5" spans="3:13">
+      <c r="C5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="3:13">
+      <c r="C6" s="2">
+        <v>21</v>
+      </c>
+      <c r="D6" s="2">
+        <v>6</v>
+      </c>
+      <c r="E6" s="2">
+        <v>160</v>
+      </c>
+      <c r="F6" s="2">
+        <v>110</v>
+      </c>
+      <c r="G6" s="2">
+        <v>3.9</v>
+      </c>
+      <c r="H6" s="2">
+        <v>2.62</v>
+      </c>
+      <c r="I6" s="2">
+        <v>16.46</v>
+      </c>
+      <c r="J6" s="2">
+        <v>0</v>
+      </c>
+      <c r="K6" s="2">
+        <v>1</v>
+      </c>
+      <c r="L6" s="2">
+        <v>4</v>
+      </c>
+      <c r="M6" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="3:13">
+      <c r="C7" s="2">
+        <v>21</v>
+      </c>
+      <c r="D7" s="2">
+        <v>6</v>
+      </c>
+      <c r="E7" s="2">
+        <v>160</v>
+      </c>
+      <c r="F7" s="2">
+        <v>110</v>
+      </c>
+      <c r="G7" s="2">
+        <v>3.9</v>
+      </c>
+      <c r="H7" s="2">
+        <v>2.875</v>
+      </c>
+      <c r="I7" s="2">
+        <v>17.02</v>
+      </c>
+      <c r="J7" s="2">
+        <v>0</v>
+      </c>
+      <c r="K7" s="2">
+        <v>1</v>
+      </c>
+      <c r="L7" s="2">
+        <v>4</v>
+      </c>
+      <c r="M7" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="3:13">
+      <c r="C8" s="2">
+        <v>22.8</v>
+      </c>
+      <c r="D8" s="2">
+        <v>4</v>
+      </c>
+      <c r="E8" s="2">
+        <v>108</v>
+      </c>
+      <c r="F8" s="2">
+        <v>93</v>
+      </c>
+      <c r="G8" s="2">
+        <v>3.85</v>
+      </c>
+      <c r="H8" s="2">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="I8" s="2">
+        <v>18.61</v>
+      </c>
+      <c r="J8" s="2">
+        <v>1</v>
+      </c>
+      <c r="K8" s="2">
+        <v>1</v>
+      </c>
+      <c r="L8" s="2">
+        <v>4</v>
+      </c>
+      <c r="M8" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="3:13">
+      <c r="C9" s="2">
+        <v>21.4</v>
+      </c>
+      <c r="D9" s="2">
+        <v>6</v>
+      </c>
+      <c r="E9" s="2">
+        <v>258</v>
+      </c>
+      <c r="F9" s="2">
+        <v>110</v>
+      </c>
+      <c r="G9" s="2">
+        <v>3.08</v>
+      </c>
+      <c r="H9" s="2">
+        <v>3.2149999999999999</v>
+      </c>
+      <c r="I9" s="2">
+        <v>19.440000000000001</v>
+      </c>
+      <c r="J9" s="2">
+        <v>1</v>
+      </c>
+      <c r="K9" s="2">
+        <v>0</v>
+      </c>
+      <c r="L9" s="2">
+        <v>3</v>
+      </c>
+      <c r="M9" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="3:13">
+      <c r="C10" s="2">
+        <v>18.7</v>
+      </c>
+      <c r="D10" s="2">
+        <v>8</v>
+      </c>
+      <c r="E10" s="2">
+        <v>360</v>
+      </c>
+      <c r="F10" s="2">
+        <v>175</v>
+      </c>
+      <c r="G10" s="2">
+        <v>3.15</v>
+      </c>
+      <c r="H10" s="2">
+        <v>3.44</v>
+      </c>
+      <c r="I10" s="2">
+        <v>17.02</v>
+      </c>
+      <c r="J10" s="2">
+        <v>0</v>
+      </c>
+      <c r="K10" s="2">
+        <v>0</v>
+      </c>
+      <c r="L10" s="2">
+        <v>3</v>
+      </c>
+      <c r="M10" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="3:13">
+      <c r="C11" s="2">
+        <v>18.100000000000001</v>
+      </c>
+      <c r="D11" s="2">
+        <v>6</v>
+      </c>
+      <c r="E11" s="2">
+        <v>225</v>
+      </c>
+      <c r="F11" s="2">
+        <v>105</v>
+      </c>
+      <c r="G11" s="2">
+        <v>2.76</v>
+      </c>
+      <c r="H11" s="2">
+        <v>3.46</v>
+      </c>
+      <c r="I11" s="2">
+        <v>20.22</v>
+      </c>
+      <c r="J11" s="2">
+        <v>1</v>
+      </c>
+      <c r="K11" s="2">
+        <v>0</v>
+      </c>
+      <c r="L11" s="2">
+        <v>3</v>
+      </c>
+      <c r="M11" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="3:13">
+      <c r="C12" s="2">
+        <v>14.3</v>
+      </c>
+      <c r="D12" s="2">
+        <v>8</v>
+      </c>
+      <c r="E12" s="2">
+        <v>360</v>
+      </c>
+      <c r="F12" s="2">
+        <v>245</v>
+      </c>
+      <c r="G12" s="2">
+        <v>3.21</v>
+      </c>
+      <c r="H12" s="2">
+        <v>3.57</v>
+      </c>
+      <c r="I12" s="2">
+        <v>15.84</v>
+      </c>
+      <c r="J12" s="2">
+        <v>0</v>
+      </c>
+      <c r="K12" s="2">
+        <v>0</v>
+      </c>
+      <c r="L12" s="2">
+        <v>3</v>
+      </c>
+      <c r="M12" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="3:13">
+      <c r="C13" s="2">
+        <v>24.4</v>
+      </c>
+      <c r="D13" s="2">
+        <v>4</v>
+      </c>
+      <c r="E13" s="2">
+        <v>146.69999999999999</v>
+      </c>
+      <c r="F13" s="2">
+        <v>62</v>
+      </c>
+      <c r="G13" s="2">
+        <v>3.69</v>
+      </c>
+      <c r="H13" s="2">
+        <v>3.19</v>
+      </c>
+      <c r="I13" s="2">
+        <v>20</v>
+      </c>
+      <c r="J13" s="2">
+        <v>1</v>
+      </c>
+      <c r="K13" s="2">
+        <v>0</v>
+      </c>
+      <c r="L13" s="2">
+        <v>4</v>
+      </c>
+      <c r="M13" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="3:13">
+      <c r="C14" s="2">
+        <v>22.8</v>
+      </c>
+      <c r="D14" s="2">
+        <v>4</v>
+      </c>
+      <c r="E14" s="2">
+        <v>140.80000000000001</v>
+      </c>
+      <c r="F14" s="2">
+        <v>95</v>
+      </c>
+      <c r="G14" s="2">
+        <v>3.92</v>
+      </c>
+      <c r="H14" s="2">
+        <v>3.15</v>
+      </c>
+      <c r="I14" s="2">
+        <v>22.9</v>
+      </c>
+      <c r="J14" s="2">
+        <v>1</v>
+      </c>
+      <c r="K14" s="2">
+        <v>0</v>
+      </c>
+      <c r="L14" s="2">
+        <v>4</v>
+      </c>
+      <c r="M14" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="3:13">
+      <c r="C15" s="2">
+        <v>19.2</v>
+      </c>
+      <c r="D15" s="2">
+        <v>6</v>
+      </c>
+      <c r="E15" s="2">
+        <v>167.6</v>
+      </c>
+      <c r="F15" s="2">
+        <v>123</v>
+      </c>
+      <c r="G15" s="2">
+        <v>3.92</v>
+      </c>
+      <c r="H15" s="2">
+        <v>3.44</v>
+      </c>
+      <c r="I15" s="2">
+        <v>18.3</v>
+      </c>
+      <c r="J15" s="2">
+        <v>1</v>
+      </c>
+      <c r="K15" s="2">
+        <v>0</v>
+      </c>
+      <c r="L15" s="2">
+        <v>4</v>
+      </c>
+      <c r="M15" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="3:13">
+      <c r="C16" s="2">
+        <v>17.8</v>
+      </c>
+      <c r="D16" s="2">
+        <v>6</v>
+      </c>
+      <c r="E16" s="2">
+        <v>167.6</v>
+      </c>
+      <c r="F16" s="2">
+        <v>123</v>
+      </c>
+      <c r="G16" s="2">
+        <v>3.92</v>
+      </c>
+      <c r="H16" s="2">
+        <v>3.44</v>
+      </c>
+      <c r="I16" s="2">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="J16" s="2">
+        <v>1</v>
+      </c>
+      <c r="K16" s="2">
+        <v>0</v>
+      </c>
+      <c r="L16" s="2">
+        <v>4</v>
+      </c>
+      <c r="M16" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="3:13">
+      <c r="C17" s="2">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="D17" s="2">
+        <v>8</v>
+      </c>
+      <c r="E17" s="2">
+        <v>275.8</v>
+      </c>
+      <c r="F17" s="2">
+        <v>180</v>
+      </c>
+      <c r="G17" s="2">
+        <v>3.07</v>
+      </c>
+      <c r="H17" s="2">
+        <v>4.07</v>
+      </c>
+      <c r="I17" s="2">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="J17" s="2">
+        <v>0</v>
+      </c>
+      <c r="K17" s="2">
+        <v>0</v>
+      </c>
+      <c r="L17" s="2">
+        <v>3</v>
+      </c>
+      <c r="M17" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="3:13">
+      <c r="C18" s="2">
+        <v>17.3</v>
+      </c>
+      <c r="D18" s="2">
+        <v>8</v>
+      </c>
+      <c r="E18" s="2">
+        <v>275.8</v>
+      </c>
+      <c r="F18" s="2">
+        <v>180</v>
+      </c>
+      <c r="G18" s="2">
+        <v>3.07</v>
+      </c>
+      <c r="H18" s="2">
+        <v>3.73</v>
+      </c>
+      <c r="I18" s="2">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="J18" s="2">
+        <v>0</v>
+      </c>
+      <c r="K18" s="2">
+        <v>0</v>
+      </c>
+      <c r="L18" s="2">
+        <v>3</v>
+      </c>
+      <c r="M18" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="3:13">
+      <c r="C19" s="2">
+        <v>15.2</v>
+      </c>
+      <c r="D19" s="2">
+        <v>8</v>
+      </c>
+      <c r="E19" s="2">
+        <v>275.8</v>
+      </c>
+      <c r="F19" s="2">
+        <v>180</v>
+      </c>
+      <c r="G19" s="2">
+        <v>3.07</v>
+      </c>
+      <c r="H19" s="2">
+        <v>3.78</v>
+      </c>
+      <c r="I19" s="2">
+        <v>18</v>
+      </c>
+      <c r="J19" s="2">
+        <v>0</v>
+      </c>
+      <c r="K19" s="2">
+        <v>0</v>
+      </c>
+      <c r="L19" s="2">
+        <v>3</v>
+      </c>
+      <c r="M19" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="3:13">
+      <c r="C20" s="2">
+        <v>10.4</v>
+      </c>
+      <c r="D20" s="2">
+        <v>8</v>
+      </c>
+      <c r="E20" s="2">
+        <v>472</v>
+      </c>
+      <c r="F20" s="2">
+        <v>205</v>
+      </c>
+      <c r="G20" s="2">
+        <v>2.93</v>
+      </c>
+      <c r="H20" s="2">
+        <v>5.25</v>
+      </c>
+      <c r="I20" s="2">
+        <v>17.98</v>
+      </c>
+      <c r="J20" s="2">
+        <v>0</v>
+      </c>
+      <c r="K20" s="2">
+        <v>0</v>
+      </c>
+      <c r="L20" s="2">
+        <v>3</v>
+      </c>
+      <c r="M20" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="3:13">
+      <c r="C21" s="2">
+        <v>10.4</v>
+      </c>
+      <c r="D21" s="2">
+        <v>8</v>
+      </c>
+      <c r="E21" s="2">
+        <v>460</v>
+      </c>
+      <c r="F21" s="2">
+        <v>215</v>
+      </c>
+      <c r="G21" s="2">
+        <v>3</v>
+      </c>
+      <c r="H21" s="2">
+        <v>5.4240000000000004</v>
+      </c>
+      <c r="I21" s="2">
+        <v>17.82</v>
+      </c>
+      <c r="J21" s="2">
+        <v>0</v>
+      </c>
+      <c r="K21" s="2">
+        <v>0</v>
+      </c>
+      <c r="L21" s="2">
+        <v>3</v>
+      </c>
+      <c r="M21" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="3:13">
+      <c r="C22" s="2">
+        <v>14.7</v>
+      </c>
+      <c r="D22" s="2">
+        <v>8</v>
+      </c>
+      <c r="E22" s="2">
+        <v>440</v>
+      </c>
+      <c r="F22" s="2">
+        <v>230</v>
+      </c>
+      <c r="G22" s="2">
+        <v>3.23</v>
+      </c>
+      <c r="H22" s="2">
+        <v>5.3449999999999998</v>
+      </c>
+      <c r="I22" s="2">
+        <v>17.420000000000002</v>
+      </c>
+      <c r="J22" s="2">
+        <v>0</v>
+      </c>
+      <c r="K22" s="2">
+        <v>0</v>
+      </c>
+      <c r="L22" s="2">
+        <v>3</v>
+      </c>
+      <c r="M22" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="3:13">
+      <c r="C23" s="2">
+        <v>32.4</v>
+      </c>
+      <c r="D23" s="2">
+        <v>4</v>
+      </c>
+      <c r="E23" s="2">
+        <v>78.7</v>
+      </c>
+      <c r="F23" s="2">
+        <v>66</v>
+      </c>
+      <c r="G23" s="2">
+        <v>4.08</v>
+      </c>
+      <c r="H23" s="2">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="I23" s="2">
+        <v>19.47</v>
+      </c>
+      <c r="J23" s="2">
+        <v>1</v>
+      </c>
+      <c r="K23" s="2">
+        <v>1</v>
+      </c>
+      <c r="L23" s="2">
+        <v>4</v>
+      </c>
+      <c r="M23" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="3:13">
+      <c r="C24" s="2">
+        <v>30.4</v>
+      </c>
+      <c r="D24" s="2">
+        <v>4</v>
+      </c>
+      <c r="E24" s="2">
+        <v>75.7</v>
+      </c>
+      <c r="F24" s="2">
+        <v>52</v>
+      </c>
+      <c r="G24" s="2">
+        <v>4.93</v>
+      </c>
+      <c r="H24" s="2">
+        <v>1.615</v>
+      </c>
+      <c r="I24" s="2">
+        <v>18.52</v>
+      </c>
+      <c r="J24" s="2">
+        <v>1</v>
+      </c>
+      <c r="K24" s="2">
+        <v>1</v>
+      </c>
+      <c r="L24" s="2">
+        <v>4</v>
+      </c>
+      <c r="M24" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="3:13">
+      <c r="C25" s="2">
+        <v>33.9</v>
+      </c>
+      <c r="D25" s="2">
+        <v>4</v>
+      </c>
+      <c r="E25" s="2">
+        <v>71.099999999999994</v>
+      </c>
+      <c r="F25" s="2">
+        <v>65</v>
+      </c>
+      <c r="G25" s="2">
+        <v>4.22</v>
+      </c>
+      <c r="H25" s="2">
+        <v>1.835</v>
+      </c>
+      <c r="I25" s="2">
+        <v>19.899999999999999</v>
+      </c>
+      <c r="J25" s="2">
+        <v>1</v>
+      </c>
+      <c r="K25" s="2">
+        <v>1</v>
+      </c>
+      <c r="L25" s="2">
+        <v>4</v>
+      </c>
+      <c r="M25" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="3:13">
+      <c r="C26" s="2">
+        <v>21.5</v>
+      </c>
+      <c r="D26" s="2">
+        <v>4</v>
+      </c>
+      <c r="E26" s="2">
+        <v>120.1</v>
+      </c>
+      <c r="F26" s="2">
+        <v>97</v>
+      </c>
+      <c r="G26" s="2">
+        <v>3.7</v>
+      </c>
+      <c r="H26" s="2">
+        <v>2.4649999999999999</v>
+      </c>
+      <c r="I26" s="2">
+        <v>20.010000000000002</v>
+      </c>
+      <c r="J26" s="2">
+        <v>1</v>
+      </c>
+      <c r="K26" s="2">
+        <v>0</v>
+      </c>
+      <c r="L26" s="2">
+        <v>3</v>
+      </c>
+      <c r="M26" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="3:13">
+      <c r="C27" s="2">
+        <v>15.5</v>
+      </c>
+      <c r="D27" s="2">
+        <v>8</v>
+      </c>
+      <c r="E27" s="2">
+        <v>318</v>
+      </c>
+      <c r="F27" s="2">
+        <v>150</v>
+      </c>
+      <c r="G27" s="2">
+        <v>2.76</v>
+      </c>
+      <c r="H27" s="2">
+        <v>3.52</v>
+      </c>
+      <c r="I27" s="2">
+        <v>16.87</v>
+      </c>
+      <c r="J27" s="2">
+        <v>0</v>
+      </c>
+      <c r="K27" s="2">
+        <v>0</v>
+      </c>
+      <c r="L27" s="2">
+        <v>3</v>
+      </c>
+      <c r="M27" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="3:13">
+      <c r="C28" s="2">
+        <v>15.2</v>
+      </c>
+      <c r="D28" s="2">
+        <v>8</v>
+      </c>
+      <c r="E28" s="2">
+        <v>304</v>
+      </c>
+      <c r="F28" s="2">
+        <v>150</v>
+      </c>
+      <c r="G28" s="2">
+        <v>3.15</v>
+      </c>
+      <c r="H28" s="2">
+        <v>3.4350000000000001</v>
+      </c>
+      <c r="I28" s="2">
+        <v>17.3</v>
+      </c>
+      <c r="J28" s="2">
+        <v>0</v>
+      </c>
+      <c r="K28" s="2">
+        <v>0</v>
+      </c>
+      <c r="L28" s="2">
+        <v>3</v>
+      </c>
+      <c r="M28" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="3:13">
+      <c r="C29" s="2">
+        <v>13.3</v>
+      </c>
+      <c r="D29" s="2">
+        <v>8</v>
+      </c>
+      <c r="E29" s="2">
+        <v>350</v>
+      </c>
+      <c r="F29" s="2">
+        <v>245</v>
+      </c>
+      <c r="G29" s="2">
+        <v>3.73</v>
+      </c>
+      <c r="H29" s="2">
+        <v>3.84</v>
+      </c>
+      <c r="I29" s="2">
+        <v>15.41</v>
+      </c>
+      <c r="J29" s="2">
+        <v>0</v>
+      </c>
+      <c r="K29" s="2">
+        <v>0</v>
+      </c>
+      <c r="L29" s="2">
+        <v>3</v>
+      </c>
+      <c r="M29" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="3:13">
+      <c r="C30" s="2">
+        <v>19.2</v>
+      </c>
+      <c r="D30" s="2">
+        <v>8</v>
+      </c>
+      <c r="E30" s="2">
+        <v>400</v>
+      </c>
+      <c r="F30" s="2">
+        <v>175</v>
+      </c>
+      <c r="G30" s="2">
+        <v>3.08</v>
+      </c>
+      <c r="H30" s="2">
+        <v>3.8450000000000002</v>
+      </c>
+      <c r="I30" s="2">
+        <v>17.05</v>
+      </c>
+      <c r="J30" s="2">
+        <v>0</v>
+      </c>
+      <c r="K30" s="2">
+        <v>0</v>
+      </c>
+      <c r="L30" s="2">
+        <v>3</v>
+      </c>
+      <c r="M30" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="3:13">
+      <c r="C31" s="2">
+        <v>27.3</v>
+      </c>
+      <c r="D31" s="2">
+        <v>4</v>
+      </c>
+      <c r="E31" s="2">
+        <v>79</v>
+      </c>
+      <c r="F31" s="2">
+        <v>66</v>
+      </c>
+      <c r="G31" s="2">
+        <v>4.08</v>
+      </c>
+      <c r="H31" s="2">
+        <v>1.9350000000000001</v>
+      </c>
+      <c r="I31" s="2">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="J31" s="2">
+        <v>1</v>
+      </c>
+      <c r="K31" s="2">
+        <v>1</v>
+      </c>
+      <c r="L31" s="2">
+        <v>4</v>
+      </c>
+      <c r="M31" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="3:13">
+      <c r="C32" s="2">
+        <v>26</v>
+      </c>
+      <c r="D32" s="2">
+        <v>4</v>
+      </c>
+      <c r="E32" s="2">
+        <v>120.3</v>
+      </c>
+      <c r="F32" s="2">
+        <v>91</v>
+      </c>
+      <c r="G32" s="2">
+        <v>4.43</v>
+      </c>
+      <c r="H32" s="2">
+        <v>2.14</v>
+      </c>
+      <c r="I32" s="2">
+        <v>16.7</v>
+      </c>
+      <c r="J32" s="2">
+        <v>0</v>
+      </c>
+      <c r="K32" s="2">
+        <v>1</v>
+      </c>
+      <c r="L32" s="2">
+        <v>5</v>
+      </c>
+      <c r="M32" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="3:13">
+      <c r="C33" s="2">
+        <v>30.4</v>
+      </c>
+      <c r="D33" s="2">
+        <v>4</v>
+      </c>
+      <c r="E33" s="2">
+        <v>95.1</v>
+      </c>
+      <c r="F33" s="2">
+        <v>113</v>
+      </c>
+      <c r="G33" s="2">
+        <v>3.77</v>
+      </c>
+      <c r="H33" s="2">
+        <v>1.5129999999999999</v>
+      </c>
+      <c r="I33" s="2">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="J33" s="2">
+        <v>1</v>
+      </c>
+      <c r="K33" s="2">
+        <v>1</v>
+      </c>
+      <c r="L33" s="2">
+        <v>5</v>
+      </c>
+      <c r="M33" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="3:13">
+      <c r="C34" s="2">
+        <v>15.8</v>
+      </c>
+      <c r="D34" s="2">
+        <v>8</v>
+      </c>
+      <c r="E34" s="2">
+        <v>351</v>
+      </c>
+      <c r="F34" s="2">
+        <v>264</v>
+      </c>
+      <c r="G34" s="2">
+        <v>4.22</v>
+      </c>
+      <c r="H34" s="2">
+        <v>3.17</v>
+      </c>
+      <c r="I34" s="2">
+        <v>14.5</v>
+      </c>
+      <c r="J34" s="2">
+        <v>0</v>
+      </c>
+      <c r="K34" s="2">
+        <v>1</v>
+      </c>
+      <c r="L34" s="2">
+        <v>5</v>
+      </c>
+      <c r="M34" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="3:13">
+      <c r="C35" s="2">
+        <v>19.7</v>
+      </c>
+      <c r="D35" s="2">
+        <v>6</v>
+      </c>
+      <c r="E35" s="2">
+        <v>145</v>
+      </c>
+      <c r="F35" s="2">
+        <v>175</v>
+      </c>
+      <c r="G35" s="2">
+        <v>3.62</v>
+      </c>
+      <c r="H35" s="2">
+        <v>2.77</v>
+      </c>
+      <c r="I35" s="2">
+        <v>15.5</v>
+      </c>
+      <c r="J35" s="2">
+        <v>0</v>
+      </c>
+      <c r="K35" s="2">
+        <v>1</v>
+      </c>
+      <c r="L35" s="2">
+        <v>5</v>
+      </c>
+      <c r="M35" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="3:13">
+      <c r="C36" s="2">
+        <v>15</v>
+      </c>
+      <c r="D36" s="2">
+        <v>8</v>
+      </c>
+      <c r="E36" s="2">
+        <v>301</v>
+      </c>
+      <c r="F36" s="2">
+        <v>335</v>
+      </c>
+      <c r="G36" s="2">
+        <v>3.54</v>
+      </c>
+      <c r="H36" s="2">
+        <v>3.57</v>
+      </c>
+      <c r="I36" s="2">
+        <v>14.6</v>
+      </c>
+      <c r="J36" s="2">
+        <v>0</v>
+      </c>
+      <c r="K36" s="2">
+        <v>1</v>
+      </c>
+      <c r="L36" s="2">
+        <v>5</v>
+      </c>
+      <c r="M36" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="3:13">
+      <c r="C37" s="2">
+        <v>21.4</v>
+      </c>
+      <c r="D37" s="2">
+        <v>4</v>
+      </c>
+      <c r="E37" s="2">
+        <v>121</v>
+      </c>
+      <c r="F37" s="2">
+        <v>109</v>
+      </c>
+      <c r="G37" s="2">
+        <v>4.1100000000000003</v>
+      </c>
+      <c r="H37" s="2">
+        <v>2.78</v>
+      </c>
+      <c r="I37" s="2">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="J37" s="2">
+        <v>1</v>
+      </c>
+      <c r="K37" s="2">
+        <v>1</v>
+      </c>
+      <c r="L37" s="2">
+        <v>4</v>
+      </c>
+      <c r="M37" s="2">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>